<commit_message>
Cập nhật data.xlsx từ công cụ QR
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>id</t>
   </si>
@@ -55,6 +55,36 @@
     <t>pinHash</t>
   </si>
   <si>
+    <t>3ojnubbo1h6</t>
+  </si>
+  <si>
+    <t>jh64ga9d</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Phường Tăng Nhơn Phú, Thành phố Hồ Chí Minh, 71300, Việt Nam</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/search/?api=1&amp;query=10.839061,106.792777</t>
+  </si>
+  <si>
+    <t>2025-08-22T09:34:12.618Z</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Phan Minh Khải</t>
+  </si>
+  <si>
+    <t>c5e29bf64454a22f</t>
+  </si>
+  <si>
+    <t>2b93044ba18dd5aab233797be33ff611a3ddd62f00c9bd241013c86ffff2ae4c</t>
+  </si>
+  <si>
     <t>szftt0p9akg</t>
   </si>
   <si>
@@ -131,9 +161,6 @@
   </si>
   <si>
     <t>Demo User</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -510,7 +537,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -593,69 +620,113 @@
         <v>20</v>
       </c>
       <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" t="s">
         <v>32</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="s">
+      <c r="K3" t="s">
         <v>34</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>35</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>36</v>
       </c>
-      <c r="J3" t="s">
+      <c r="N3" t="s">
         <v>37</v>
       </c>
-      <c r="K3" t="s">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="L3" t="s">
+      <c r="B4" t="s">
         <v>39</v>
       </c>
-      <c r="M3" t="s">
+      <c r="C4" t="s">
         <v>40</v>
       </c>
-      <c r="N3" t="s">
-        <v>40</v>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>